<commit_message>
24 - test read excel
</commit_message>
<xml_diff>
--- a/data/groups.xlsx
+++ b/data/groups.xlsx
@@ -18,19 +18,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>nameSJ&lt;c42 Q5</t>
+    <t>namen</t>
   </si>
   <si>
-    <t xml:space="preserve">name`nFT/ </t>
+    <t>namekJ-uw&gt;</t>
   </si>
   <si>
-    <t>name</t>
+    <t>name?S0y sFT3</t>
   </si>
   <si>
-    <t>name_.]J{41</t>
+    <t>name*</t>
   </si>
   <si>
-    <t xml:space="preserve">namev </t>
+    <t>nameuUPC</t>
   </si>
 </sst>
 </file>

</xml_diff>